<commit_message>
2 major bugs fixed | 1) SRA arthmetic shift (not circular shift) | 2) lh sign extension bug | emulator has the near to golden simulator
</commit_message>
<xml_diff>
--- a/riscv/instructions.xlsx
+++ b/riscv/instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCSU_classes_files\spring20\633\Project\HMP\Heterogeneous-multicore\riscv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50A691BE-6E26-4D7E-ADAC-4C3828D801DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF84650-01C5-45F3-A8F9-D67E9689C324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,9 +547,6 @@
     <t>sra rd rs1 imm</t>
   </si>
   <si>
-    <t>GPR[rd] = {GPR[rs1], GPR[rs1]} &gt;&gt; GPR[rs2][4:0]</t>
-  </si>
-  <si>
     <t>or rd rs1 rs2</t>
   </si>
   <si>
@@ -635,9 +632,6 @@
   </si>
   <si>
     <t>srai rd rs1 imm</t>
-  </si>
-  <si>
-    <t>GPR[rd] = {GPR[rs1], GPR[rs1]} &gt;&gt; signex[imm][4:0]</t>
   </si>
   <si>
     <t>I-type - Load Instns</t>
@@ -1033,6 +1027,12 @@
   </si>
   <si>
     <t>0xac020054</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] &gt;&gt;&gt; GPR[rs2][4:0]</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] &gt;&gt;&gt; signex[imm][4:0]</t>
   </si>
 </sst>
 </file>
@@ -1272,6 +1272,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1287,7 +1290,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1295,12 +1301,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1686,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,14 +1839,14 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="20" t="s">
         <v>91</v>
       </c>
@@ -1858,23 +1858,23 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="10" t="s">
         <v>81</v>
       </c>
@@ -1900,7 +1900,7 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="5" t="s">
         <v>87</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>165</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>166</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2211,10 +2211,10 @@
         <v>117</v>
       </c>
       <c r="I23" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2243,10 +2243,10 @@
         <v>119</v>
       </c>
       <c r="I24" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2259,30 +2259,30 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B26" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
+      <c r="B26" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
       <c r="M26" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="C27" s="33"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" s="34"/>
       <c r="D27" s="10" t="s">
         <v>83</v>
       </c>
@@ -2302,11 +2302,11 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="34" t="s">
+      <c r="A28" s="32"/>
+      <c r="B28" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="34"/>
+      <c r="C28" s="35"/>
       <c r="D28" s="5" t="s">
         <v>89</v>
       </c>
@@ -2378,13 +2378,13 @@
         <v>122</v>
       </c>
       <c r="H30" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I30" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="J30" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2408,13 +2408,13 @@
         <v>122</v>
       </c>
       <c r="H31" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="J31" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2438,13 +2438,13 @@
         <v>122</v>
       </c>
       <c r="H32" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I32" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="J32" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2468,13 +2468,13 @@
         <v>122</v>
       </c>
       <c r="H33" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="J33" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2498,13 +2498,13 @@
         <v>122</v>
       </c>
       <c r="H34" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="I34" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="J34" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2530,13 +2530,13 @@
         <v>122</v>
       </c>
       <c r="H35" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I35" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="J35" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2562,13 +2562,13 @@
         <v>122</v>
       </c>
       <c r="H36" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="J36" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2594,13 +2594,13 @@
         <v>122</v>
       </c>
       <c r="H37" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="I37" s="4" t="s">
-        <v>195</v>
-      </c>
       <c r="J37" s="4" t="s">
-        <v>196</v>
+        <v>321</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2613,27 +2613,27 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B39" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
+      <c r="B39" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="C40" s="33"/>
+      <c r="A40" s="32"/>
+      <c r="B40" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="34"/>
       <c r="D40" s="10" t="s">
         <v>83</v>
       </c>
@@ -2651,15 +2651,15 @@
         <v>107</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="34" t="s">
+      <c r="A41" s="32"/>
+      <c r="B41" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="34"/>
+      <c r="C41" s="35"/>
       <c r="D41" s="5" t="s">
         <v>89</v>
       </c>
@@ -2701,13 +2701,13 @@
         <v>126</v>
       </c>
       <c r="H42" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="J42" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2731,13 +2731,13 @@
         <v>126</v>
       </c>
       <c r="H43" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J43" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2767,7 +2767,7 @@
         <v>127</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2791,10 +2791,10 @@
         <v>126</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>128</v>
@@ -2821,13 +2821,13 @@
         <v>126</v>
       </c>
       <c r="H46" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J46" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2842,27 +2842,27 @@
       <c r="J47" s="13"/>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
+      <c r="B48" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="33"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
-      <c r="B49" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="C49" s="33"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="34"/>
       <c r="D49" s="10" t="s">
         <v>83</v>
       </c>
@@ -2880,11 +2880,11 @@
         <v>107</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="5" t="s">
         <v>96</v>
       </c>
@@ -2934,13 +2934,13 @@
         <v>129</v>
       </c>
       <c r="H51" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="J51" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -2966,13 +2966,13 @@
         <v>129</v>
       </c>
       <c r="H52" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="J52" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3004,7 +3004,7 @@
         <v>130</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -3026,23 +3026,23 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B56" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
-      <c r="H56" s="34"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="34"/>
+      <c r="B56" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="35"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="31"/>
+      <c r="A57" s="32"/>
       <c r="B57" s="10" t="s">
         <v>81</v>
       </c>
@@ -3068,7 +3068,7 @@
       <c r="J57" s="10"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
+      <c r="A58" s="32"/>
       <c r="B58" s="20" t="s">
         <v>132</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>142</v>
       </c>
       <c r="J58" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -3126,7 +3126,7 @@
         <v>134</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3152,13 +3152,13 @@
         <v>133</v>
       </c>
       <c r="H60" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="J60" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -3184,13 +3184,13 @@
         <v>133</v>
       </c>
       <c r="H61" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="J61" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -3216,13 +3216,13 @@
         <v>133</v>
       </c>
       <c r="H62" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="J62" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -3248,13 +3248,13 @@
         <v>133</v>
       </c>
       <c r="H63" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="J63" s="4" t="s">
         <v>231</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -3280,13 +3280,13 @@
         <v>133</v>
       </c>
       <c r="H64" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="J64" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -3308,23 +3308,23 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="34" t="s">
-        <v>237</v>
-      </c>
-      <c r="C67" s="34"/>
-      <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="34"/>
-      <c r="H67" s="34"/>
-      <c r="I67" s="34"/>
-      <c r="J67" s="34"/>
+      <c r="B67" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="35"/>
+      <c r="H67" s="35"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="35"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="31"/>
+      <c r="A68" s="32"/>
       <c r="B68" s="10" t="s">
         <v>81</v>
       </c>
@@ -3350,15 +3350,15 @@
       <c r="J68" s="10"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
-      <c r="B69" s="35" t="s">
+      <c r="A69" s="32"/>
+      <c r="B69" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C69" s="35"/>
-      <c r="D69" s="35" t="s">
+      <c r="C69" s="36"/>
+      <c r="D69" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="E69" s="35"/>
+      <c r="E69" s="36"/>
       <c r="F69" s="25" t="s">
         <v>91</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>142</v>
       </c>
       <c r="J69" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -3400,31 +3400,31 @@
         <v>138</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="31" t="s">
+      <c r="A72" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B72" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="32"/>
-      <c r="H72" s="32"/>
-      <c r="I72" s="32"/>
-      <c r="J72" s="32"/>
+      <c r="B72" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C72" s="33"/>
+      <c r="D72" s="33"/>
+      <c r="E72" s="33"/>
+      <c r="F72" s="33"/>
+      <c r="G72" s="33"/>
+      <c r="H72" s="33"/>
+      <c r="I72" s="33"/>
+      <c r="J72" s="33"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
-      <c r="B73" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="C73" s="33"/>
+      <c r="A73" s="32"/>
+      <c r="B73" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="C73" s="34"/>
       <c r="D73" s="10" t="s">
         <v>83</v>
       </c>
@@ -3444,11 +3444,11 @@
       <c r="J73" s="10"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
-      <c r="B74" s="34" t="s">
+      <c r="A74" s="32"/>
+      <c r="B74" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C74" s="34"/>
+      <c r="C74" s="35"/>
       <c r="D74" s="5" t="s">
         <v>89</v>
       </c>
@@ -3487,42 +3487,42 @@
         <v>91</v>
       </c>
       <c r="G75" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I75" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H75" s="4" t="s">
+      <c r="J75" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="I75" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>243</v>
-      </c>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="31" t="s">
+      <c r="A77" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B77" s="32" t="s">
+      <c r="B77" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="32"/>
-      <c r="G77" s="32"/>
-      <c r="H77" s="32"/>
-      <c r="I77" s="32"/>
-      <c r="J77" s="32"/>
+      <c r="C77" s="33"/>
+      <c r="D77" s="33"/>
+      <c r="E77" s="33"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="33"/>
+      <c r="H77" s="33"/>
+      <c r="I77" s="33"/>
+      <c r="J77" s="33"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="31"/>
-      <c r="B78" s="33" t="s">
+      <c r="A78" s="32"/>
+      <c r="B78" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="C78" s="33"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="33"/>
+      <c r="C78" s="34"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="34"/>
       <c r="F78" s="10" t="s">
         <v>85</v>
       </c>
@@ -3536,13 +3536,13 @@
       <c r="J78" s="10"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="31"/>
-      <c r="B79" s="34" t="s">
+      <c r="A79" s="32"/>
+      <c r="B79" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C79" s="34"/>
-      <c r="D79" s="34"/>
-      <c r="E79" s="34"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
+      <c r="E79" s="35"/>
       <c r="F79" s="5" t="s">
         <v>91</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>142</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -3573,16 +3573,16 @@
         <v>91</v>
       </c>
       <c r="G80" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I80" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="H80" s="4" t="s">
+      <c r="J80" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="J80" s="4" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -3599,41 +3599,39 @@
         <v>91</v>
       </c>
       <c r="G81" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="I81" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="H81" s="4" t="s">
+      <c r="J81" s="4" t="s">
         <v>250</v>
-      </c>
-      <c r="I81" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>252</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:J39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="B77:J77"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:J72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:J56"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:J67"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:E69"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -3641,25 +3639,27 @@
     <mergeCell ref="A48:A50"/>
     <mergeCell ref="B48:J48"/>
     <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:J56"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:J67"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B72:J72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="B77:J77"/>
-    <mergeCell ref="B78:E78"/>
-    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3689,18 +3689,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -3948,18 +3948,18 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -3986,20 +3986,20 @@
       <c r="I12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="33" t="s">
+      <c r="J12" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33" t="s">
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33" t="s">
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="Q12" s="33"/>
+      <c r="Q12" s="34"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
@@ -4048,14 +4048,14 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
@@ -4071,25 +4071,25 @@
       <c r="F15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33" t="s">
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33" t="s">
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33" t="s">
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="Q15" s="33"/>
+      <c r="Q15" s="34"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
@@ -4237,14 +4237,14 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="11"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
@@ -4254,27 +4254,27 @@
       <c r="D21" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33" t="s">
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33" t="s">
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33" t="s">
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="Q21" s="33"/>
+      <c r="Q21" s="34"/>
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
@@ -4298,20 +4298,20 @@
       </c>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
-      <c r="M22" s="37" t="s">
+      <c r="M22" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="38" t="s">
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="Q22" s="38"/>
+      <c r="Q22" s="40"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C24" s="15" t="s">
@@ -4458,17 +4458,29 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="C11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="P22:Q23"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:Q18"/>
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="M15:O15"/>
@@ -4477,29 +4489,17 @@
     <mergeCell ref="J16:L16"/>
     <mergeCell ref="M16:O16"/>
     <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="P22:Q23"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="P12:Q12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4663,14 +4663,14 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="20" t="s">
         <v>91</v>
       </c>
@@ -4860,10 +4860,10 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="34"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="5" t="s">
         <v>89</v>
       </c>
@@ -5054,14 +5054,14 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36" t="s">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="36"/>
+      <c r="E31" s="31"/>
       <c r="F31" s="20" t="s">
         <v>91</v>
       </c>
@@ -5099,17 +5099,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5136,19 +5136,19 @@
   <sheetData>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="D4" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="E4" s="26" t="s">
         <v>255</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>256</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>257</v>
       </c>
       <c r="F4" s="18">
         <v>0</v>
@@ -5234,31 +5234,31 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="27">
         <v>0</v>
       </c>
       <c r="E5" t="s">
+        <v>258</v>
+      </c>
+      <c r="F5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G5" t="s">
         <v>260</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>261</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>262</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>263</v>
-      </c>
-      <c r="I5" t="s">
-        <v>264</v>
-      </c>
-      <c r="J5" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -5266,31 +5266,31 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D6" s="27">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H6" t="s">
+        <v>260</v>
+      </c>
+      <c r="I6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J6" t="s">
         <v>262</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>263</v>
-      </c>
-      <c r="J6" t="s">
-        <v>264</v>
-      </c>
-      <c r="K6" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -5298,31 +5298,31 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D7" s="27">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H7" t="s">
+        <v>259</v>
+      </c>
+      <c r="I7" t="s">
+        <v>260</v>
+      </c>
+      <c r="J7" t="s">
         <v>261</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>262</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>263</v>
-      </c>
-      <c r="K7" t="s">
-        <v>264</v>
-      </c>
-      <c r="L7" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -5330,31 +5330,31 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>273</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>276</v>
-      </c>
       <c r="I8" t="s">
+        <v>259</v>
+      </c>
+      <c r="J8" t="s">
+        <v>260</v>
+      </c>
+      <c r="K8" t="s">
         <v>261</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>262</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>263</v>
-      </c>
-      <c r="L8" t="s">
-        <v>264</v>
-      </c>
-      <c r="M8" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -5362,31 +5362,31 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D9" s="27">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J9" t="s">
+        <v>259</v>
+      </c>
+      <c r="K9" t="s">
+        <v>260</v>
+      </c>
+      <c r="L9" t="s">
         <v>261</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>262</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>263</v>
-      </c>
-      <c r="M9" t="s">
-        <v>264</v>
-      </c>
-      <c r="N9" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -5394,31 +5394,31 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D10" s="27">
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K10" t="s">
+        <v>259</v>
+      </c>
+      <c r="L10" t="s">
+        <v>260</v>
+      </c>
+      <c r="M10" t="s">
         <v>261</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>262</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>263</v>
-      </c>
-      <c r="N10" t="s">
-        <v>264</v>
-      </c>
-      <c r="O10" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -5426,34 +5426,34 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D11" s="27">
         <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L11" t="s">
+        <v>259</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="N11" t="s">
+        <v>260</v>
+      </c>
+      <c r="O11" t="s">
         <v>261</v>
       </c>
-      <c r="M11" s="18" t="s">
+      <c r="P11" t="s">
         <v>262</v>
       </c>
-      <c r="N11" t="s">
-        <v>262</v>
-      </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>263</v>
-      </c>
-      <c r="P11" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -5461,34 +5461,34 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
+        <v>284</v>
+      </c>
+      <c r="C12" t="s">
+        <v>285</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>287</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="E12" t="s">
-        <v>289</v>
-      </c>
       <c r="M12" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="N12" t="s">
+        <v>259</v>
+      </c>
+      <c r="O12" t="s">
+        <v>260</v>
+      </c>
+      <c r="P12" t="s">
         <v>261</v>
       </c>
-      <c r="N12" t="s">
-        <v>261</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>262</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>263</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>264</v>
-      </c>
-      <c r="R12" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -5496,34 +5496,34 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D13" s="27">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="O13" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="P13" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>260</v>
+      </c>
+      <c r="R13" t="s">
         <v>261</v>
       </c>
-      <c r="P13" t="s">
+      <c r="S13" t="s">
         <v>262</v>
       </c>
-      <c r="Q13" t="s">
-        <v>262</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>263</v>
-      </c>
-      <c r="S13" t="s">
-        <v>264</v>
-      </c>
-      <c r="T13" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -5531,16 +5531,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D14" s="29">
         <v>24</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
@@ -5554,19 +5554,19 @@
       <c r="O14" s="29"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="R14" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="S14" s="29" t="s">
         <v>261</v>
       </c>
-      <c r="R14" s="29" t="s">
+      <c r="T14" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="S14" s="29" t="s">
+      <c r="U14" s="29" t="s">
         <v>263</v>
-      </c>
-      <c r="T14" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="U14" s="29" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -5574,34 +5574,34 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D15" s="27">
         <v>28</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="Q15" s="18" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="R15" t="s">
+        <v>259</v>
+      </c>
+      <c r="S15" t="s">
+        <v>260</v>
+      </c>
+      <c r="T15" t="s">
         <v>261</v>
       </c>
-      <c r="S15" t="s">
+      <c r="U15" t="s">
         <v>262</v>
       </c>
-      <c r="T15" t="s">
+      <c r="V15" t="s">
         <v>263</v>
-      </c>
-      <c r="U15" t="s">
-        <v>264</v>
-      </c>
-      <c r="V15" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -5609,31 +5609,31 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
+        <v>298</v>
+      </c>
+      <c r="C16" t="s">
+        <v>299</v>
+      </c>
+      <c r="D16" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>301</v>
       </c>
-      <c r="D16" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="E16" t="s">
-        <v>303</v>
-      </c>
       <c r="S16" t="s">
+        <v>259</v>
+      </c>
+      <c r="T16" t="s">
+        <v>260</v>
+      </c>
+      <c r="U16" t="s">
         <v>261</v>
       </c>
-      <c r="T16" t="s">
+      <c r="V16" t="s">
         <v>262</v>
       </c>
-      <c r="U16" t="s">
+      <c r="W16" t="s">
         <v>263</v>
-      </c>
-      <c r="V16" t="s">
-        <v>264</v>
-      </c>
-      <c r="W16" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
@@ -5641,31 +5641,31 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C17" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D17" s="27">
         <v>30</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="T17" t="s">
+        <v>259</v>
+      </c>
+      <c r="U17" t="s">
+        <v>260</v>
+      </c>
+      <c r="V17" t="s">
         <v>261</v>
       </c>
-      <c r="U17" t="s">
+      <c r="W17" t="s">
         <v>262</v>
       </c>
-      <c r="V17" t="s">
+      <c r="X17" t="s">
         <v>263</v>
-      </c>
-      <c r="W17" t="s">
-        <v>264</v>
-      </c>
-      <c r="X17" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
@@ -5673,31 +5673,31 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C18" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D18" s="27">
         <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="U18" t="s">
+        <v>259</v>
+      </c>
+      <c r="V18" t="s">
+        <v>260</v>
+      </c>
+      <c r="W18" t="s">
         <v>261</v>
       </c>
-      <c r="V18" t="s">
+      <c r="X18" t="s">
         <v>262</v>
       </c>
-      <c r="W18" t="s">
+      <c r="Y18" t="s">
         <v>263</v>
-      </c>
-      <c r="X18" t="s">
-        <v>264</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
@@ -5705,31 +5705,31 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C19" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D19" s="27">
         <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="V19" t="s">
+        <v>259</v>
+      </c>
+      <c r="W19" t="s">
+        <v>260</v>
+      </c>
+      <c r="X19" t="s">
         <v>261</v>
       </c>
-      <c r="W19" t="s">
+      <c r="Y19" t="s">
         <v>262</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Z19" t="s">
         <v>263</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>264</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -5737,31 +5737,31 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
+        <v>311</v>
+      </c>
+      <c r="C20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="E20" t="s">
         <v>313</v>
       </c>
-      <c r="C20" t="s">
-        <v>291</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="E20" t="s">
-        <v>315</v>
-      </c>
       <c r="W20" t="s">
+        <v>259</v>
+      </c>
+      <c r="X20" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y20" t="s">
         <v>261</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Z20" t="s">
         <v>262</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="AA20" t="s">
         <v>263</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>264</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
@@ -5769,16 +5769,16 @@
         <v>17</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D21" s="29">
         <v>40</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
@@ -5799,19 +5799,19 @@
       <c r="V21" s="29"/>
       <c r="W21" s="29"/>
       <c r="X21" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y21" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z21" s="29" t="s">
         <v>261</v>
       </c>
-      <c r="Y21" s="29" t="s">
+      <c r="AA21" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="Z21" s="29" t="s">
+      <c r="AB21" s="29" t="s">
         <v>263</v>
-      </c>
-      <c r="AA21" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="AB21" s="29" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
@@ -5819,34 +5819,34 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C22" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D22" s="27">
         <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="X22" s="18" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="Y22" t="s">
+        <v>259</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>260</v>
+      </c>
+      <c r="AA22" t="s">
         <v>261</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AB22" t="s">
         <v>262</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AC22" t="s">
         <v>263</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>264</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>